<commit_message>
Retrained the model. Addressing issue #15
</commit_message>
<xml_diff>
--- a/04_Safety_Helmet_Vest_Detection/Safety_helmet_vest_img/exe/yolov3/yolov3_summary.xlsx
+++ b/04_Safety_Helmet_Vest_Detection/Safety_helmet_vest_img/exe/yolov3/yolov3_summary.xlsx
@@ -5745,7 +5745,7 @@
         <v>13</v>
       </c>
       <c r="O88" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="P88" t="n">
         <v>13</v>
@@ -5754,7 +5754,7 @@
         <v>13</v>
       </c>
       <c r="S88" t="n">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="89" outlineLevel="1">
@@ -6285,7 +6285,7 @@
         <v>26</v>
       </c>
       <c r="O97" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="P97" t="n">
         <v>26</v>
@@ -6294,7 +6294,7 @@
         <v>26</v>
       </c>
       <c r="S97" t="n">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="98" outlineLevel="1">
@@ -6825,7 +6825,7 @@
         <v>52</v>
       </c>
       <c r="O106" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="P106" t="n">
         <v>52</v>
@@ -6834,7 +6834,7 @@
         <v>52</v>
       </c>
       <c r="S106" t="n">
-        <v>484</v>
+        <v>469</v>
       </c>
     </row>
     <row r="107" outlineLevel="1">
@@ -6873,7 +6873,7 @@
         <v>0</v>
       </c>
       <c r="L107" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="M107" t="n">
         <v>13</v>
@@ -6882,7 +6882,7 @@
         <v>13</v>
       </c>
       <c r="O107" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="P107" t="n">
         <v>13</v>
@@ -6891,7 +6891,7 @@
         <v>13</v>
       </c>
       <c r="S107" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="108" outlineLevel="1">
@@ -6930,7 +6930,7 @@
         <v>0</v>
       </c>
       <c r="L108" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="M108" t="n">
         <v>13</v>
@@ -6939,7 +6939,7 @@
         <v>13</v>
       </c>
       <c r="O108" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="P108" t="n">
         <v>13</v>
@@ -6948,7 +6948,7 @@
         <v>13</v>
       </c>
       <c r="S108" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="109" outlineLevel="1">
@@ -6987,7 +6987,7 @@
         <v>0</v>
       </c>
       <c r="L109" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="M109" t="n">
         <v>26</v>
@@ -6996,7 +6996,7 @@
         <v>26</v>
       </c>
       <c r="O109" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="P109" t="n">
         <v>26</v>
@@ -7005,7 +7005,7 @@
         <v>26</v>
       </c>
       <c r="S109" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="110" outlineLevel="1">
@@ -7044,7 +7044,7 @@
         <v>0</v>
       </c>
       <c r="L110" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="M110" t="n">
         <v>26</v>
@@ -7053,7 +7053,7 @@
         <v>26</v>
       </c>
       <c r="O110" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="P110" t="n">
         <v>26</v>
@@ -7062,7 +7062,7 @@
         <v>26</v>
       </c>
       <c r="S110" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="111" outlineLevel="1">
@@ -7101,7 +7101,7 @@
         <v>0</v>
       </c>
       <c r="L111" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="M111" t="n">
         <v>52</v>
@@ -7110,7 +7110,7 @@
         <v>52</v>
       </c>
       <c r="O111" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="P111" t="n">
         <v>52</v>
@@ -7119,7 +7119,7 @@
         <v>52</v>
       </c>
       <c r="S111" t="n">
-        <v>77</v>
+        <v>54</v>
       </c>
     </row>
     <row r="112" outlineLevel="1">
@@ -7158,7 +7158,7 @@
         <v>0</v>
       </c>
       <c r="L112" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="M112" t="n">
         <v>52</v>
@@ -7167,7 +7167,7 @@
         <v>52</v>
       </c>
       <c r="O112" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="P112" t="n">
         <v>52</v>
@@ -7176,7 +7176,7 @@
         <v>52</v>
       </c>
       <c r="S112" t="n">
-        <v>64</v>
+        <v>45</v>
       </c>
     </row>
     <row r="113" outlineLevel="1">
@@ -7189,7 +7189,7 @@
         </is>
       </c>
       <c r="S113" t="n">
-        <v>188963</v>
+        <v>188888</v>
       </c>
     </row>
     <row r="114">

</xml_diff>